<commit_message>
update and add styles
</commit_message>
<xml_diff>
--- a/rates.xlsx
+++ b/rates.xlsx
@@ -16,14 +16,20 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="1">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
+    <numFmt numFmtId="165" formatCode="dd.mm.yy"/>
+  </numFmts>
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -46,8 +52,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -126,7 +137,7 @@
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
-  <style val="13"/>
+  <style val="12"/>
   <chart>
     <title>
       <tx>
@@ -178,12 +189,12 @@
           </marker>
           <cat>
             <numRef>
-              <f>'EUR exchange rate'!$A$2:$A$13</f>
+              <f>'EUR exchange rate'!$A$2:$A$37</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'EUR exchange rate'!$B$2:$B$13</f>
+              <f>'EUR exchange rate'!$B$2:$B$37</f>
             </numRef>
           </val>
         </ser>
@@ -196,7 +207,22 @@
           <orientation val="minMax"/>
         </scaling>
         <axPos val="l"/>
-        <numFmt formatCode="dd.mm.yy" sourceLinked="0"/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>Date</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <numFmt formatCode="dd.mm.yyyy" sourceLinked="0"/>
         <majorTickMark val="none"/>
         <minorTickMark val="none"/>
         <crossAx val="100"/>
@@ -247,7 +273,7 @@
       <row>0</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="7200000" cy="3600000"/>
+    <ext cx="9000000" cy="3600000"/>
     <graphicFrame>
       <nvGraphicFramePr>
         <cNvPr id="1" name="Chart 1"/>
@@ -554,144 +580,315 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:B37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="12" customWidth="1" min="1" max="1"/>
+  </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" t="inlineStr">
+      <c r="A1" s="1" t="inlineStr">
         <is>
           <t>Date</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
+      <c r="B1" s="1" t="inlineStr">
         <is>
           <t>EUR</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>01.01.2021</t>
-        </is>
-      </c>
-      <c r="B2" t="n">
+      <c r="A2" s="2" t="n">
+        <v>44197</v>
+      </c>
+      <c r="B2" s="3" t="n">
         <v>34.97</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>01.02.2021</t>
-        </is>
-      </c>
-      <c r="B3" t="n">
+      <c r="A3" s="2" t="n">
+        <v>44228</v>
+      </c>
+      <c r="B3" s="3" t="n">
         <v>34.2</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>01.03.2021</t>
-        </is>
-      </c>
-      <c r="B4" t="n">
+      <c r="A4" s="2" t="n">
+        <v>44256</v>
+      </c>
+      <c r="B4" s="3" t="n">
         <v>33.9</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>01.04.2021</t>
-        </is>
-      </c>
-      <c r="B5" t="n">
+      <c r="A5" s="2" t="n">
+        <v>44287</v>
+      </c>
+      <c r="B5" s="3" t="n">
         <v>32.85</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>01.05.2021</t>
-        </is>
-      </c>
-      <c r="B6" t="n">
+      <c r="A6" s="2" t="n">
+        <v>44317</v>
+      </c>
+      <c r="B6" s="3" t="n">
         <v>33.75</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>01.06.2021</t>
-        </is>
-      </c>
-      <c r="B7" t="n">
+      <c r="A7" s="2" t="n">
+        <v>44348</v>
+      </c>
+      <c r="B7" s="3" t="n">
         <v>33.7</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>01.07.2021</t>
-        </is>
-      </c>
-      <c r="B8" t="n">
+      <c r="A8" s="2" t="n">
+        <v>44378</v>
+      </c>
+      <c r="B8" s="3" t="n">
         <v>32.6</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>01.08.2021</t>
-        </is>
-      </c>
-      <c r="B9" t="n">
+      <c r="A9" s="2" t="n">
+        <v>44409</v>
+      </c>
+      <c r="B9" s="3" t="n">
         <v>32.2</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>01.09.2021</t>
-        </is>
-      </c>
-      <c r="B10" t="n">
+      <c r="A10" s="2" t="n">
+        <v>44440</v>
+      </c>
+      <c r="B10" s="3" t="n">
         <v>32.15</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>01.10.2021</t>
-        </is>
-      </c>
-      <c r="B11" t="n">
+      <c r="A11" s="2" t="n">
+        <v>44470</v>
+      </c>
+      <c r="B11" s="3" t="n">
         <v>31.1</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>01.11.2021</t>
-        </is>
-      </c>
-      <c r="B12" t="n">
+      <c r="A12" s="2" t="n">
+        <v>44501</v>
+      </c>
+      <c r="B12" s="3" t="n">
         <v>30.7</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>01.12.2021</t>
-        </is>
-      </c>
-      <c r="B13" t="n">
+      <c r="A13" s="2" t="n">
+        <v>44531</v>
+      </c>
+      <c r="B13" s="3" t="n">
         <v>31.1</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="2" t="n">
+        <v>44562</v>
+      </c>
+      <c r="B14" s="3" t="n">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="2" t="n">
+        <v>44593</v>
+      </c>
+      <c r="B15" s="3" t="n">
+        <v>32.2</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="2" t="n">
+        <v>44621</v>
+      </c>
+      <c r="B16" s="3" t="n">
+        <v>33.3</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="2" t="n">
+        <v>44652</v>
+      </c>
+      <c r="B17" s="3" t="n">
+        <v>32.75</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="2" t="n">
+        <v>44682</v>
+      </c>
+      <c r="B18" s="3" t="n">
+        <v>33.8</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="2" t="n">
+        <v>44713</v>
+      </c>
+      <c r="B19" s="3" t="n">
+        <v>38.3</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="2" t="n">
+        <v>44743</v>
+      </c>
+      <c r="B20" s="3" t="n">
+        <v>37.4</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="2" t="n">
+        <v>44774</v>
+      </c>
+      <c r="B21" s="3" t="n">
+        <v>40.8</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="2" t="n">
+        <v>44805</v>
+      </c>
+      <c r="B22" s="3" t="n">
+        <v>40.5</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="2" t="n">
+        <v>44835</v>
+      </c>
+      <c r="B23" s="3" t="n">
+        <v>40.8</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="2" t="n">
+        <v>44866</v>
+      </c>
+      <c r="B24" s="3" t="n">
+        <v>39.4</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="2" t="n">
+        <v>44896</v>
+      </c>
+      <c r="B25" s="3" t="n">
+        <v>41.3</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="2" t="n">
+        <v>44927</v>
+      </c>
+      <c r="B26" s="3" t="n">
+        <v>42.45</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="2" t="n">
+        <v>44958</v>
+      </c>
+      <c r="B27" s="3" t="n">
+        <v>43.4</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="2" t="n">
+        <v>44986</v>
+      </c>
+      <c r="B28" s="3" t="n">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="2" t="n">
+        <v>45017</v>
+      </c>
+      <c r="B29" s="3" t="n">
+        <v>40.9</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="2" t="n">
+        <v>45047</v>
+      </c>
+      <c r="B30" s="3" t="n">
+        <v>41.6</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="2" t="n">
+        <v>45078</v>
+      </c>
+      <c r="B31" s="3" t="n">
+        <v>40.5</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="2" t="n">
+        <v>45108</v>
+      </c>
+      <c r="B32" s="3" t="n">
+        <v>41.1</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="2" t="n">
+        <v>45139</v>
+      </c>
+      <c r="B33" s="3" t="n">
+        <v>41.55</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="2" t="n">
+        <v>45170</v>
+      </c>
+      <c r="B34" s="3" t="n">
+        <v>41.6</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="2" t="n">
+        <v>45200</v>
+      </c>
+      <c r="B35" s="3" t="n">
+        <v>40.8</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="2" t="n">
+        <v>45231</v>
+      </c>
+      <c r="B36" s="3" t="n">
+        <v>40.25</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="2" t="n">
+        <v>45261</v>
+      </c>
+      <c r="B37" s="3" t="n">
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>